<commit_message>
feat: :sparkles: mas de un periodo ademas de validacion de semestre y carrera
</commit_message>
<xml_diff>
--- a/static/docs/carreras.xlsx
+++ b/static/docs/carreras.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos_cunoc\Modela2\GESTOR\static\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\Cargar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5589E57-3B33-46BF-ABCD-0299AB89D67F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED8444A-AE88-4BBF-AD49-195956BE2F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{29F2FEF8-74CD-481E-98CD-BBE344CC6849}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>codigo</t>
   </si>
@@ -78,6 +78,27 @@
   </si>
   <si>
     <t>C006</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>2257B9</t>
+  </si>
+  <si>
+    <t>22B949</t>
+  </si>
+  <si>
+    <t>22B9B7</t>
+  </si>
+  <si>
+    <t>22B964</t>
+  </si>
+  <si>
+    <t>E9A660</t>
+  </si>
+  <si>
+    <t>5D63EA</t>
   </si>
 </sst>
 </file>
@@ -119,10 +140,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,7 +460,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A7"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,6 +472,9 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -460,7 +483,9 @@
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -470,7 +495,9 @@
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -480,7 +507,9 @@
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -490,7 +519,9 @@
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -500,7 +531,9 @@
       <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -510,7 +543,9 @@
       <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
   </sheetData>

</xml_diff>